<commit_message>
Update terminal storage amounts in "input_param" files
Update terminal storage amounts for compressed and liquid hydrogen in "input_param" files to work with code update. Rerun analysis script.
</commit_message>
<xml_diff>
--- a/systems2atoms/systems/inputs/input_params_Pd_4nm.xlsx
+++ b/systems2atoms/systems/inputs/input_params_Pd_4nm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/modeling/model - LOCAL COPY/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doellnl-my.sharepoint.com/personal/yuan13_llnl_gov/Documents/Documents/_work/projects/System to Atoms (S2A)/GitHub/systems2atoms/systems2atoms/systems/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1BCEEF4-1A4D-436F-B2C3-F0A3B057FFD8}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:40009_{386061FE-3CDD-48D5-AA75-D7117555D095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1127A725-65BD-4903-8F8B-7DA14588C879}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{E2D57577-FB13-429E-AB3B-629C91C7C3A5}">
+    <comment ref="AL1" authorId="0" shapeId="0" xr:uid="{E2D57577-FB13-429E-AB3B-629C91C7C3A5}">
       <text>
         <r>
           <rPr>
@@ -382,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{6762015A-B38C-4887-9CF1-D4DFF7E78527}">
+    <comment ref="AM1" authorId="0" shapeId="0" xr:uid="{6762015A-B38C-4887-9CF1-D4DFF7E78527}">
       <text>
         <r>
           <rPr>
@@ -585,7 +585,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>run #</t>
   </si>
@@ -708,6 +708,12 @@
   </si>
   <si>
     <t>electro</t>
+  </si>
+  <si>
+    <t>terminal compressed hydrogen storage amount (days)</t>
+  </si>
+  <si>
+    <t>terminal liquid hydrogen storage amount (days)</t>
   </si>
 </sst>
 </file>
@@ -1298,10 +1304,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1601,19 +1603,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL56"/>
+  <dimension ref="A1:AN56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -1638,20 +1640,22 @@
     <col min="25" max="25" width="31" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="50" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="31" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="29" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="43" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="43" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1734,40 +1738,46 @@
         <v>37</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1850,40 +1860,46 @@
         <v>0.25</v>
       </c>
       <c r="AB2" s="1">
-        <v>300</v>
+        <v>0.25</v>
       </c>
       <c r="AC2" s="1">
         <v>1</v>
       </c>
       <c r="AD2" s="1">
+        <v>300</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="1">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AG2" s="1">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AH2" s="1">
         <v>1</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AI2" s="1">
         <v>9.6467120334224301</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AJ2" s="1">
         <v>3500</v>
       </c>
-      <c r="AI2" s="1">
+      <c r="AK2" s="1">
         <v>1</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AL2" s="1">
         <v>0</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AM2" s="1">
         <v>0</v>
       </c>
-      <c r="AL2" s="1">
+      <c r="AN2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1891,38 +1907,38 @@
         <f t="shared" ref="B3:B34" si="0">B2+1</f>
         <v>1</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>300</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>1</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>7.31028611028611E-2</v>
       </c>
-      <c r="AF3">
+      <c r="AH3">
         <v>1</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>9.6467120334224337</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>3500</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>1</v>
       </c>
-      <c r="AJ3">
+      <c r="AL3">
         <v>0</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1930,17 +1946,17 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>310.5263157894737</v>
       </c>
-      <c r="AE4">
+      <c r="AG4">
         <v>3.06770616770616E-2</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>4.0481696005543908</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1948,17 +1964,17 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>321.0526315789474</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>1.36387486387486E-2</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>1.7997801813681762</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1966,17 +1982,17 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>331.57894736842098</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>6.3794673794673696E-3</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>0.84183961896841764</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1984,17 +2000,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>342.10526315789468</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>3.12978912978913E-3</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>0.41300947739827742</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2002,17 +2018,17 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <v>352.63157894736838</v>
       </c>
-      <c r="AE8">
+      <c r="AG8">
         <v>1.5999405999406E-3</v>
       </c>
-      <c r="AG8">
+      <c r="AI8">
         <v>0.21112944152064153</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2020,17 +2036,17 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>363.15789473684208</v>
       </c>
-      <c r="AE9">
+      <c r="AG9">
         <v>8.4999324999325001E-4</v>
       </c>
-      <c r="AG9">
+      <c r="AI9">
         <v>0.11216578926370925</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2038,17 +2054,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <v>373.68421052631578</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>4.6999666999666999E-4</v>
       </c>
-      <c r="AG10">
+      <c r="AI10">
         <v>6.2021136570096565E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2056,17 +2072,17 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <v>384.21052631578948</v>
       </c>
-      <c r="AE11">
+      <c r="AG11">
         <v>2.6999846999847002E-4</v>
       </c>
-      <c r="AG11">
+      <c r="AI11">
         <v>3.5629214099774105E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2074,32 +2090,32 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="AB12">
+      <c r="AD12">
         <v>300</v>
       </c>
-      <c r="AC12">
+      <c r="AE12">
         <v>21.84210526315789</v>
       </c>
-      <c r="AD12">
+      <c r="AF12">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE12">
+      <c r="AG12">
         <v>7.6013986013985999E-2</v>
       </c>
-      <c r="AF12">
+      <c r="AH12">
         <v>1</v>
       </c>
-      <c r="AG12">
+      <c r="AI12">
         <v>10.030866405594402</v>
       </c>
-      <c r="AH12">
+      <c r="AJ12">
         <v>3500</v>
       </c>
-      <c r="AI12">
+      <c r="AK12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -2107,17 +2123,17 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="AB13">
+      <c r="AD13">
         <v>310.5263157894737</v>
       </c>
-      <c r="AE13">
+      <c r="AG13">
         <v>3.1048951048951001E-2</v>
       </c>
-      <c r="AG13">
+      <c r="AI13">
         <v>4.097244419580413</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2125,17 +2141,17 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="AB14">
+      <c r="AD14">
         <v>321.0526315789474</v>
       </c>
-      <c r="AE14">
+      <c r="AG14">
         <v>1.3516483516483499E-2</v>
       </c>
-      <c r="AG14">
+      <c r="AI14">
         <v>1.7836459780219758</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2143,17 +2159,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="AB15">
+      <c r="AD15">
         <v>331.57894736842098</v>
       </c>
-      <c r="AE15">
+      <c r="AG15">
         <v>6.1994851994851899E-3</v>
       </c>
-      <c r="AG15">
+      <c r="AI15">
         <v>0.81808902651222526</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2161,17 +2177,17 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="AB16">
+      <c r="AD16">
         <v>342.10526315789468</v>
       </c>
-      <c r="AE16">
+      <c r="AG16">
         <v>2.9798039798039702E-3</v>
       </c>
-      <c r="AG16">
+      <c r="AI16">
         <v>0.39321731701811574</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2179,17 +2195,17 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="AB17">
+      <c r="AD17">
         <v>352.63157894736838</v>
       </c>
-      <c r="AE17">
+      <c r="AG17">
         <v>1.4999504999504999E-3</v>
       </c>
-      <c r="AG17">
+      <c r="AI17">
         <v>0.19793466793386794</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -2197,17 +2213,17 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AB18">
+      <c r="AD18">
         <v>363.15789473684208</v>
       </c>
-      <c r="AE18">
+      <c r="AG18">
         <v>7.8999378999379001E-4</v>
       </c>
-      <c r="AG18">
+      <c r="AI18">
         <v>0.10424821252261253</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2215,17 +2231,17 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="AB19">
+      <c r="AD19">
         <v>373.68421052631578</v>
       </c>
-      <c r="AE19">
+      <c r="AG19">
         <v>4.2396792396792298E-4</v>
       </c>
-      <c r="AG19">
+      <c r="AI19">
         <v>5.5947146421146288E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2233,17 +2249,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AB20">
+      <c r="AD20">
         <v>384.21052631578948</v>
       </c>
-      <c r="AE20">
+      <c r="AG20">
         <v>2.3798633798633701E-4</v>
       </c>
-      <c r="AG20">
+      <c r="AI20">
         <v>3.1404867549747424E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2251,32 +2267,32 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="AB21">
+      <c r="AD21">
         <v>300</v>
       </c>
-      <c r="AC21">
+      <c r="AE21">
         <v>42.684210526315788</v>
       </c>
-      <c r="AD21">
+      <c r="AF21">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE21">
+      <c r="AG21">
         <v>7.6013986013985999E-2</v>
       </c>
-      <c r="AF21">
+      <c r="AH21">
         <v>1</v>
       </c>
-      <c r="AG21">
+      <c r="AI21">
         <v>10.030866405594402</v>
       </c>
-      <c r="AH21">
+      <c r="AJ21">
         <v>3500</v>
       </c>
-      <c r="AI21">
+      <c r="AK21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2284,17 +2300,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="AB22">
+      <c r="AD22">
         <v>310.5263157894737</v>
       </c>
-      <c r="AE22">
+      <c r="AG22">
         <v>3.11388611388611E-2</v>
       </c>
-      <c r="AG22">
+      <c r="AI22">
         <v>4.1091090269730213</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2302,17 +2318,17 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="AB23">
+      <c r="AD23">
         <v>321.0526315789474</v>
       </c>
-      <c r="AE23">
+      <c r="AG23">
         <v>1.3496503496503401E-2</v>
       </c>
-      <c r="AG23">
+      <c r="AI23">
         <v>1.7810093986013857</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -2320,17 +2336,17 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AB24">
+      <c r="AD24">
         <v>331.57894736842098</v>
       </c>
-      <c r="AE24">
+      <c r="AG24">
         <v>6.1753984753984701E-3</v>
       </c>
-      <c r="AG24">
+      <c r="AI24">
         <v>0.81491052313236234</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2338,17 +2354,17 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AB25">
+      <c r="AD25">
         <v>342.10526315789468</v>
       </c>
-      <c r="AE25">
+      <c r="AG25">
         <v>2.96471636471636E-3</v>
       </c>
-      <c r="AG25">
+      <c r="AI25">
         <v>0.39122634326106265</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2356,17 +2372,17 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AB26">
+      <c r="AD26">
         <v>352.63157894736838</v>
       </c>
-      <c r="AE26">
+      <c r="AG26">
         <v>1.4868626868626801E-3</v>
       </c>
-      <c r="AG26">
+      <c r="AI26">
         <v>0.19620758964854876</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2374,17 +2390,17 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AB27">
+      <c r="AD27">
         <v>363.15789473684208</v>
       </c>
-      <c r="AE27">
+      <c r="AG27">
         <v>7.7693297693297596E-4</v>
       </c>
-      <c r="AG27">
+      <c r="AI27">
         <v>0.10252469718245706</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2392,17 +2408,17 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AB28">
+      <c r="AD28">
         <v>373.68421052631578</v>
       </c>
-      <c r="AE28">
+      <c r="AG28">
         <v>4.2096822096821998E-4</v>
       </c>
-      <c r="AG28">
+      <c r="AI28">
         <v>5.5551303213543089E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -2410,17 +2426,17 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AB29">
+      <c r="AD29">
         <v>384.21052631578948</v>
       </c>
-      <c r="AE29">
+      <c r="AG29">
         <v>2.3598653598653501E-4</v>
       </c>
-      <c r="AG29">
+      <c r="AI29">
         <v>3.1140972078011947E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2428,32 +2444,32 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AB30">
+      <c r="AD30">
         <v>300</v>
       </c>
-      <c r="AC30">
+      <c r="AE30">
         <v>63.526315789473678</v>
       </c>
-      <c r="AD30">
+      <c r="AF30">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE30">
+      <c r="AG30">
         <v>7.6013986013985999E-2</v>
       </c>
-      <c r="AF30">
+      <c r="AH30">
         <v>1</v>
       </c>
-      <c r="AG30">
+      <c r="AI30">
         <v>10.030866405594402</v>
       </c>
-      <c r="AH30">
+      <c r="AJ30">
         <v>3500</v>
       </c>
-      <c r="AI30">
+      <c r="AK30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2461,17 +2477,17 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AB31">
+      <c r="AD31">
         <v>310.5263157894737</v>
       </c>
-      <c r="AE31">
+      <c r="AG31">
         <v>3.11388611388611E-2</v>
       </c>
-      <c r="AG31">
+      <c r="AI31">
         <v>4.1091090269730213</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2479,17 +2495,17 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AB32">
+      <c r="AD32">
         <v>321.0526315789474</v>
       </c>
-      <c r="AE32">
+      <c r="AG32">
         <v>1.3496503496503401E-2</v>
       </c>
-      <c r="AG32">
+      <c r="AI32">
         <v>1.7810093986013857</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -2497,17 +2513,17 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AB33">
+      <c r="AD33">
         <v>331.57894736842098</v>
       </c>
-      <c r="AE33">
+      <c r="AG33">
         <v>6.1673992673992603E-3</v>
       </c>
-      <c r="AG33">
+      <c r="AI33">
         <v>0.81385494124542024</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -2515,17 +2531,17 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AB34">
+      <c r="AD34">
         <v>342.10526315789468</v>
       </c>
-      <c r="AE34">
+      <c r="AG34">
         <v>2.9597168597168501E-3</v>
       </c>
-      <c r="AG34">
+      <c r="AI34">
         <v>0.39056660458172332</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2533,17 +2549,17 @@
         <f t="shared" ref="B35:B56" si="1">B34+1</f>
         <v>33</v>
       </c>
-      <c r="AB35">
+      <c r="AD35">
         <v>352.63157894736838</v>
       </c>
-      <c r="AE35">
+      <c r="AG35">
         <v>1.4838629838629801E-3</v>
       </c>
-      <c r="AG35">
+      <c r="AI35">
         <v>0.19581174644094593</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -2551,17 +2567,17 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="AB36">
+      <c r="AD36">
         <v>363.15789473684208</v>
       </c>
-      <c r="AE36">
+      <c r="AG36">
         <v>7.7393327393327296E-4</v>
       </c>
-      <c r="AG36">
+      <c r="AI36">
         <v>0.10212885397485384</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2569,17 +2585,17 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="AB37">
+      <c r="AD37">
         <v>373.68421052631578</v>
       </c>
-      <c r="AE37">
+      <c r="AG37">
         <v>4.1896841896841799E-4</v>
       </c>
-      <c r="AG37">
+      <c r="AI37">
         <v>5.5287407741807612E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2587,17 +2603,17 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="AB38">
+      <c r="AD38">
         <v>384.21052631578948</v>
       </c>
-      <c r="AE38">
+      <c r="AG38">
         <v>2.3498663498663401E-4</v>
       </c>
-      <c r="AG38">
+      <c r="AI38">
         <v>3.1009024342144212E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2605,32 +2621,32 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="AB39">
+      <c r="AD39">
         <v>300</v>
       </c>
-      <c r="AC39">
+      <c r="AE39">
         <v>84.368421052631575</v>
       </c>
-      <c r="AD39">
+      <c r="AF39">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE39">
+      <c r="AG39">
         <v>7.6013986013985999E-2</v>
       </c>
-      <c r="AF39">
+      <c r="AH39">
         <v>1</v>
       </c>
-      <c r="AG39">
+      <c r="AI39">
         <v>10.030866405594402</v>
       </c>
-      <c r="AH39">
+      <c r="AJ39">
         <v>3500</v>
       </c>
-      <c r="AI39">
+      <c r="AK39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2638,17 +2654,17 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="AB40">
+      <c r="AD40">
         <v>310.5263157894737</v>
       </c>
-      <c r="AE40">
+      <c r="AG40">
         <v>3.11388611388611E-2</v>
       </c>
-      <c r="AG40">
+      <c r="AI40">
         <v>4.1091090269730213</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2656,17 +2672,17 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="AB41">
+      <c r="AD41">
         <v>321.0526315789474</v>
       </c>
-      <c r="AE41">
+      <c r="AG41">
         <v>1.3496503496503401E-2</v>
       </c>
-      <c r="AG41">
+      <c r="AI41">
         <v>1.7810093986013857</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2674,17 +2690,17 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="AB42">
+      <c r="AD42">
         <v>331.57894736842098</v>
       </c>
-      <c r="AE42">
+      <c r="AG42">
         <v>6.1673992673992603E-3</v>
       </c>
-      <c r="AG42">
+      <c r="AI42">
         <v>0.81385494124542024</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -2692,17 +2708,17 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="AB43">
+      <c r="AD43">
         <v>342.10526315789468</v>
       </c>
-      <c r="AE43">
+      <c r="AG43">
         <v>2.9567171567171499E-3</v>
       </c>
-      <c r="AG43">
+      <c r="AI43">
         <v>0.39017076137412043</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -2710,17 +2726,17 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="AB44">
+      <c r="AD44">
         <v>352.63157894736838</v>
       </c>
-      <c r="AE44">
+      <c r="AG44">
         <v>1.48186318186318E-3</v>
       </c>
-      <c r="AG44">
+      <c r="AI44">
         <v>0.19554785096921071</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2728,17 +2744,17 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="AB45">
+      <c r="AD45">
         <v>363.15789473684208</v>
       </c>
-      <c r="AE45">
+      <c r="AG45">
         <v>7.7293337293337196E-4</v>
       </c>
-      <c r="AG45">
+      <c r="AI45">
         <v>0.10199690623898611</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -2746,17 +2762,17 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="AB46">
+      <c r="AD46">
         <v>373.68421052631578</v>
       </c>
-      <c r="AE46">
+      <c r="AG46">
         <v>4.1796851796851699E-4</v>
       </c>
-      <c r="AG46">
+      <c r="AI46">
         <v>5.515546000593987E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -2764,17 +2780,17 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="AB47">
+      <c r="AD47">
         <v>384.21052631578948</v>
       </c>
-      <c r="AE47">
+      <c r="AG47">
         <v>2.3398673398673301E-4</v>
       </c>
-      <c r="AG47">
+      <c r="AI47">
         <v>3.087707660627648E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -2782,32 +2798,32 @@
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="AB48">
+      <c r="AD48">
         <v>300</v>
       </c>
-      <c r="AC48">
+      <c r="AE48">
         <v>100</v>
       </c>
-      <c r="AD48">
+      <c r="AF48">
         <v>0.99990000000000001</v>
       </c>
-      <c r="AE48">
+      <c r="AG48">
         <v>7.6013986013985999E-2</v>
       </c>
-      <c r="AF48">
+      <c r="AH48">
         <v>1</v>
       </c>
-      <c r="AG48">
+      <c r="AI48">
         <v>10.030866405594402</v>
       </c>
-      <c r="AH48">
+      <c r="AJ48">
         <v>3500</v>
       </c>
-      <c r="AI48">
+      <c r="AK48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -2815,17 +2831,17 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="AB49">
+      <c r="AD49">
         <v>310.5263157894737</v>
       </c>
-      <c r="AE49">
+      <c r="AG49">
         <v>3.11388611388611E-2</v>
       </c>
-      <c r="AG49">
+      <c r="AI49">
         <v>4.1091090269730213</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -2833,17 +2849,17 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="AB50">
+      <c r="AD50">
         <v>321.0526315789474</v>
       </c>
-      <c r="AE50">
+      <c r="AG50">
         <v>1.3496503496503401E-2</v>
       </c>
-      <c r="AG50">
+      <c r="AI50">
         <v>1.7810093986013857</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -2851,17 +2867,17 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="AB51">
+      <c r="AD51">
         <v>331.57894736842098</v>
       </c>
-      <c r="AE51">
+      <c r="AG51">
         <v>6.1694881694881699E-3</v>
       </c>
-      <c r="AG51">
+      <c r="AI51">
         <v>0.8141305944361944</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -2869,17 +2885,17 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="AB52">
+      <c r="AD52">
         <v>342.10526315789468</v>
       </c>
-      <c r="AE52">
+      <c r="AG52">
         <v>2.9598059598059598E-3</v>
       </c>
-      <c r="AG52">
+      <c r="AI52">
         <v>0.39057836230076226</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -2887,17 +2903,17 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="AB53">
+      <c r="AD53">
         <v>352.63157894736838</v>
       </c>
-      <c r="AE53">
+      <c r="AG53">
         <v>1.48995148995149E-3</v>
       </c>
-      <c r="AG53">
+      <c r="AI53">
         <v>0.19661519057519058</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -2905,17 +2921,17 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="AB54">
+      <c r="AD54">
         <v>363.15789473684208</v>
       </c>
-      <c r="AE54">
+      <c r="AG54">
         <v>7.7999387999388005E-4</v>
       </c>
-      <c r="AG54">
+      <c r="AI54">
         <v>0.1029286163990964</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -2923,17 +2939,17 @@
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="AB55">
+      <c r="AD55">
         <v>373.68421052631578</v>
       </c>
-      <c r="AE55">
+      <c r="AG55">
         <v>4.1999711999712001E-4</v>
       </c>
-      <c r="AG55">
+      <c r="AI55">
         <v>5.5423155952515957E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -2941,18 +2957,18 @@
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="AB56">
+      <c r="AD56">
         <v>384.21052631578948</v>
       </c>
-      <c r="AE56">
+      <c r="AG56">
         <v>2.3398673398673301E-4</v>
       </c>
-      <c r="AG56">
+      <c r="AI56">
         <v>3.087707660627648E-2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C3:AL56">
+  <conditionalFormatting sqref="C3:AN56">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C3&lt;&gt;C$2</formula>
     </cfRule>

</xml_diff>